<commit_message>
Traduction de la page home + traduction de la page portefeuille
</commit_message>
<xml_diff>
--- a/src/main/resources/accented_chars_unicode.xlsx
+++ b/src/main/resources/accented_chars_unicode.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>Lettre</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>&amp;uuml;</t>
+  </si>
+  <si>
+    <t>°</t>
+  </si>
+  <si>
+    <t>\u00b0</t>
   </si>
 </sst>
 </file>
@@ -537,7 +543,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -718,7 +724,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="18" spans="2:2">
+    <row r="17" spans="1:2">
+      <c r="A17" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="B18" s="2"/>
     </row>
   </sheetData>

</xml_diff>